<commit_message>
lots of minor updates
</commit_message>
<xml_diff>
--- a/CEDEN/data_dictionaries/data_dictionary_conversion/chemistry/CEDEN_Chemistry_Data_Dictionary.xlsx
+++ b/CEDEN/data_dictionaries/data_dictionary_conversion/chemistry/CEDEN_Chemistry_Data_Dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\David\Open_Data_Project\__CA_DataPortal\CEDEN\data_dictionary_conversion\water_chemistry\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawaterboards-my.sharepoint.com/personal/david_altare_waterboards_ca_gov/Documents/projects/CA_data_portal/CEDEN/data_dictionaries/data_dictionary_conversion/chemistry/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFBDAF8-957E-428B-86AD-B157FC800F31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{8CFBDAF8-957E-428B-86AD-B157FC800F31}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{5784411E-664A-46EC-A0CF-0484A2CD92CD}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CEDEN_Chemistry_Data_Dictionary" sheetId="1" r:id="rId1"/>
@@ -2029,21 +2029,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="103.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="103.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="62" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="62" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
@@ -2063,7 +2063,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -2109,7 +2109,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
@@ -2133,7 +2133,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
@@ -2156,7 +2156,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="72.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="60.5" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>19</v>
       </c>
@@ -2179,7 +2179,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="36.5" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
@@ -2203,7 +2203,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>25</v>
       </c>
@@ -2226,7 +2226,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="48.5" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>28</v>
       </c>
@@ -2250,7 +2250,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>31</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>35</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="48.5" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>38</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="36.5" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>41</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>44</v>
       </c>
@@ -2366,7 +2366,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="48.5" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>47</v>
       </c>
@@ -2390,7 +2390,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="36.5" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>49</v>
       </c>
@@ -2413,7 +2413,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="36.5" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>52</v>
       </c>
@@ -2437,7 +2437,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>55</v>
       </c>
@@ -2460,7 +2460,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>58</v>
       </c>
@@ -2483,7 +2483,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="84.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>59</v>
       </c>
@@ -2507,7 +2507,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="36.5" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>61</v>
       </c>
@@ -2531,7 +2531,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>62</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="48.5" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>64</v>
       </c>
@@ -2578,7 +2578,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="48.5" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>66</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="36.5" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>68</v>
       </c>
@@ -2626,7 +2626,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="36.5" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>71</v>
       </c>
@@ -2649,7 +2649,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>74</v>
       </c>
@@ -2672,7 +2672,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="36.5" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>75</v>
       </c>
@@ -2695,7 +2695,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>78</v>
       </c>
@@ -2718,7 +2718,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>81</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>84</v>
       </c>
@@ -2764,7 +2764,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>87</v>
       </c>
@@ -2787,7 +2787,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="36.5" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>88</v>
       </c>
@@ -2811,7 +2811,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="36.5" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
         <v>91</v>
       </c>
@@ -2834,7 +2834,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>94</v>
       </c>
@@ -2857,7 +2857,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
         <v>97</v>
       </c>
@@ -2880,7 +2880,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="48.5" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
         <v>100</v>
       </c>
@@ -2903,7 +2903,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>103</v>
       </c>
@@ -2927,7 +2927,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="s">
         <v>105</v>
       </c>
@@ -2950,7 +2950,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="36.5" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
         <v>108</v>
       </c>
@@ -2973,7 +2973,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
         <v>111</v>
       </c>
@@ -2996,7 +2996,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="48.5" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
         <v>112</v>
       </c>
@@ -3021,7 +3021,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
         <v>115</v>
       </c>
@@ -3044,7 +3044,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="36.5" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
         <v>118</v>
       </c>
@@ -3068,7 +3068,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="36.5" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
         <v>120</v>
       </c>
@@ -3092,7 +3092,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
         <v>123</v>
       </c>
@@ -3115,7 +3115,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
         <v>126</v>
       </c>
@@ -3138,7 +3138,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="36.5" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
         <v>127</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="48.5" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
         <v>130</v>
       </c>
@@ -3185,7 +3185,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="36.5" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
         <v>132</v>
       </c>
@@ -3209,7 +3209,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
         <v>135</v>
       </c>
@@ -3232,7 +3232,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="48.5" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="s">
         <v>138</v>
       </c>
@@ -3255,7 +3255,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
         <v>141</v>
       </c>
@@ -3279,7 +3279,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="36.5" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="s">
         <v>143</v>
       </c>
@@ -3302,7 +3302,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
         <v>146</v>
       </c>
@@ -3326,7 +3326,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="s">
         <v>148</v>
       </c>
@@ -3349,7 +3349,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" s="4" t="s">
         <v>151</v>
       </c>
@@ -3372,7 +3372,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A58" s="4" t="s">
         <v>154</v>
       </c>
@@ -3395,7 +3395,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" s="4" t="s">
         <v>157</v>
       </c>
@@ -3418,7 +3418,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A60" s="4" t="s">
         <v>160</v>
       </c>
@@ -3441,7 +3441,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" ht="48.5" x14ac:dyDescent="0.35">
       <c r="A61" s="4" t="s">
         <v>163</v>
       </c>
@@ -3464,7 +3464,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="36.5" x14ac:dyDescent="0.35">
       <c r="A62" s="4" t="s">
         <v>166</v>
       </c>
@@ -3487,7 +3487,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A63" s="4" t="s">
         <v>169</v>
       </c>
@@ -3510,7 +3510,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A64" s="4" t="s">
         <v>172</v>
       </c>
@@ -3534,7 +3534,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" s="4" t="s">
         <v>174</v>
       </c>
@@ -3557,7 +3557,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" s="4" t="s">
         <v>177</v>
       </c>
@@ -3580,7 +3580,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A67" s="4" t="s">
         <v>180</v>
       </c>
@@ -3604,7 +3604,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" s="4" t="s">
         <v>182</v>
       </c>
@@ -3627,7 +3627,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A69" s="4" t="s">
         <v>185</v>
       </c>
@@ -3650,7 +3650,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" s="4" t="s">
         <v>188</v>
       </c>
@@ -3673,7 +3673,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" ht="132.5" x14ac:dyDescent="0.35">
       <c r="A71" s="4" t="s">
         <v>191</v>
       </c>
@@ -3704,7 +3704,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="72.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A72" s="4" t="s">
         <v>193</v>
       </c>
@@ -3730,7 +3730,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" ht="48.5" x14ac:dyDescent="0.35">
       <c r="A73" s="4" t="s">
         <v>196</v>
       </c>
@@ -3772,20 +3772,20 @@
   <dimension ref="A1:E68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="11.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="28" style="9" customWidth="1"/>
     <col min="2" max="2" width="16" style="9" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="114.28515625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" style="58" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="9"/>
+    <col min="3" max="3" width="9.26953125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="114.26953125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="9.26953125" style="58" customWidth="1"/>
+    <col min="6" max="16384" width="9.1796875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="12" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>198</v>
       </c>
@@ -3802,7 +3802,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>172</v>
       </c>
@@ -3820,7 +3820,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>81</v>
       </c>
@@ -3838,7 +3838,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="A4" s="18" t="s">
         <v>31</v>
       </c>
@@ -3856,7 +3856,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="36" x14ac:dyDescent="0.35">
       <c r="A5" s="21" t="s">
         <v>108</v>
       </c>
@@ -3874,7 +3874,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="48" x14ac:dyDescent="0.35">
       <c r="A6" s="25" t="s">
         <v>100</v>
       </c>
@@ -3892,7 +3892,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="A7" s="29" t="s">
         <v>41</v>
       </c>
@@ -3910,7 +3910,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="A8" s="30" t="s">
         <v>25</v>
       </c>
@@ -3928,7 +3928,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="36" x14ac:dyDescent="0.35">
       <c r="A9" s="29" t="s">
         <v>75</v>
       </c>
@@ -3946,7 +3946,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="132" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="126.5" x14ac:dyDescent="0.35">
       <c r="A10" s="30" t="s">
         <v>191</v>
       </c>
@@ -3964,7 +3964,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="72" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="69" x14ac:dyDescent="0.35">
       <c r="A11" s="29" t="s">
         <v>193</v>
       </c>
@@ -3982,7 +3982,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="46" x14ac:dyDescent="0.35">
       <c r="A12" s="30" t="s">
         <v>196</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="A13" s="29" t="s">
         <v>123</v>
       </c>
@@ -4018,7 +4018,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A14" s="30" t="s">
         <v>120</v>
       </c>
@@ -4036,7 +4036,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="36" x14ac:dyDescent="0.35">
       <c r="A15" s="29" t="s">
         <v>127</v>
       </c>
@@ -4054,7 +4054,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="A16" s="30" t="s">
         <v>146</v>
       </c>
@@ -4072,7 +4072,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="A17" s="29" t="s">
         <v>177</v>
       </c>
@@ -4090,7 +4090,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="12" x14ac:dyDescent="0.35">
       <c r="A18" s="30" t="s">
         <v>188</v>
       </c>
@@ -4108,7 +4108,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A19" s="43" t="s">
         <v>88</v>
       </c>
@@ -4126,7 +4126,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="36" x14ac:dyDescent="0.35">
       <c r="A20" s="30" t="s">
         <v>130</v>
       </c>
@@ -4144,7 +4144,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="12" x14ac:dyDescent="0.35">
       <c r="A21" s="29" t="s">
         <v>97</v>
       </c>
@@ -4162,7 +4162,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="48" x14ac:dyDescent="0.35">
       <c r="A22" s="45" t="s">
         <v>163</v>
       </c>
@@ -4180,7 +4180,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="A23" s="46" t="s">
         <v>166</v>
       </c>
@@ -4198,7 +4198,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A24" s="47" t="s">
         <v>132</v>
       </c>
@@ -4216,7 +4216,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="48" x14ac:dyDescent="0.35">
       <c r="A25" s="48" t="s">
         <v>47</v>
       </c>
@@ -4234,7 +4234,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="36" x14ac:dyDescent="0.35">
       <c r="A26" s="49" t="s">
         <v>49</v>
       </c>
@@ -4252,7 +4252,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="A27" s="50" t="s">
         <v>103</v>
       </c>
@@ -4270,7 +4270,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="46" x14ac:dyDescent="0.35">
       <c r="A28" s="49" t="s">
         <v>28</v>
       </c>
@@ -4288,7 +4288,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="A29" s="21" t="s">
         <v>182</v>
       </c>
@@ -4306,7 +4306,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="A30" s="51" t="s">
         <v>169</v>
       </c>
@@ -4324,7 +4324,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="12" x14ac:dyDescent="0.35">
       <c r="A31" s="43" t="s">
         <v>105</v>
       </c>
@@ -4342,7 +4342,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A32" s="30" t="s">
         <v>52</v>
       </c>
@@ -4360,7 +4360,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="48" x14ac:dyDescent="0.35">
       <c r="A33" s="29" t="s">
         <v>64</v>
       </c>
@@ -4378,7 +4378,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="A34" s="30" t="s">
         <v>55</v>
       </c>
@@ -4396,7 +4396,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="12" x14ac:dyDescent="0.35">
       <c r="A35" s="43" t="s">
         <v>62</v>
       </c>
@@ -4414,7 +4414,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="A36" s="30" t="s">
         <v>141</v>
       </c>
@@ -4432,7 +4432,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="A37" s="29" t="s">
         <v>10</v>
       </c>
@@ -4450,7 +4450,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="46" x14ac:dyDescent="0.35">
       <c r="A38" s="30" t="s">
         <v>112</v>
       </c>
@@ -4468,7 +4468,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="A39" s="29" t="s">
         <v>118</v>
       </c>
@@ -4486,7 +4486,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="A40" s="54" t="s">
         <v>115</v>
       </c>
@@ -4504,7 +4504,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="A41" s="29" t="s">
         <v>6</v>
       </c>
@@ -4522,7 +4522,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="23" x14ac:dyDescent="0.35">
       <c r="A42" s="55" t="s">
         <v>13</v>
       </c>
@@ -4540,7 +4540,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="36" x14ac:dyDescent="0.35">
       <c r="A43" s="29" t="s">
         <v>91</v>
       </c>
@@ -4558,7 +4558,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="36" x14ac:dyDescent="0.35">
       <c r="A44" s="30" t="s">
         <v>71</v>
       </c>
@@ -4576,7 +4576,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="36" x14ac:dyDescent="0.35">
       <c r="A45" s="29" t="s">
         <v>68</v>
       </c>
@@ -4594,7 +4594,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="36" x14ac:dyDescent="0.35">
       <c r="A46" s="55" t="s">
         <v>61</v>
       </c>
@@ -4612,7 +4612,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="12" x14ac:dyDescent="0.35">
       <c r="A47" s="43" t="s">
         <v>84</v>
       </c>
@@ -4630,7 +4630,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="A48" s="30" t="s">
         <v>44</v>
       </c>
@@ -4648,7 +4648,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="48" x14ac:dyDescent="0.35">
       <c r="A49" s="29" t="s">
         <v>66</v>
       </c>
@@ -4666,7 +4666,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="A50" s="30" t="s">
         <v>94</v>
       </c>
@@ -4684,7 +4684,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="12" x14ac:dyDescent="0.35">
       <c r="A51" s="29" t="s">
         <v>78</v>
       </c>
@@ -4702,7 +4702,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="36" x14ac:dyDescent="0.35">
       <c r="A52" s="30" t="s">
         <v>22</v>
       </c>
@@ -4720,7 +4720,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="A53" s="43" t="s">
         <v>185</v>
       </c>
@@ -4738,7 +4738,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A54" s="30" t="s">
         <v>38</v>
       </c>
@@ -4756,7 +4756,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="A55" s="29" t="s">
         <v>143</v>
       </c>
@@ -4774,7 +4774,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" ht="60" x14ac:dyDescent="0.35">
       <c r="A56" s="30" t="s">
         <v>19</v>
       </c>
@@ -4792,7 +4792,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="A57" s="29" t="s">
         <v>16</v>
       </c>
@@ -4810,7 +4810,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" ht="12" x14ac:dyDescent="0.35">
       <c r="A58" s="30" t="s">
         <v>157</v>
       </c>
@@ -4828,7 +4828,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" ht="12" x14ac:dyDescent="0.35">
       <c r="A59" s="29" t="s">
         <v>151</v>
       </c>
@@ -4846,7 +4846,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="48" x14ac:dyDescent="0.35">
       <c r="A60" s="30" t="s">
         <v>138</v>
       </c>
@@ -4864,7 +4864,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="A61" s="29" t="s">
         <v>135</v>
       </c>
@@ -4882,7 +4882,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="A62" s="30" t="s">
         <v>180</v>
       </c>
@@ -4900,7 +4900,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="72" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A63" s="29" t="s">
         <v>59</v>
       </c>
@@ -4918,7 +4918,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="A64" s="30" t="s">
         <v>35</v>
       </c>
@@ -4936,7 +4936,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="A65" s="21" t="s">
         <v>148</v>
       </c>
@@ -4954,7 +4954,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="A66" s="57" t="s">
         <v>160</v>
       </c>
@@ -4972,7 +4972,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="A67" s="29" t="s">
         <v>154</v>
       </c>
@@ -4990,7 +4990,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" ht="12" x14ac:dyDescent="0.35">
       <c r="A68" s="55" t="s">
         <v>174</v>
       </c>
@@ -5057,9 +5057,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5073,7 +5073,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -5081,7 +5081,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -5089,7 +5089,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -5097,7 +5097,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -5105,7 +5105,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -5113,7 +5113,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -5121,7 +5121,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -5129,7 +5129,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -5137,7 +5137,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -5145,7 +5145,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -5153,7 +5153,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -5161,7 +5161,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -5169,7 +5169,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -5177,7 +5177,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -5185,7 +5185,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>49</v>
       </c>
@@ -5193,7 +5193,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -5201,7 +5201,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>55</v>
       </c>
@@ -5209,7 +5209,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>58</v>
       </c>
@@ -5217,7 +5217,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>59</v>
       </c>
@@ -5225,7 +5225,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>61</v>
       </c>
@@ -5233,7 +5233,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>62</v>
       </c>
@@ -5241,7 +5241,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>64</v>
       </c>
@@ -5249,7 +5249,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>66</v>
       </c>
@@ -5257,7 +5257,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>68</v>
       </c>
@@ -5265,7 +5265,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>71</v>
       </c>
@@ -5273,7 +5273,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>74</v>
       </c>
@@ -5281,7 +5281,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>75</v>
       </c>
@@ -5289,7 +5289,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>78</v>
       </c>
@@ -5297,7 +5297,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>81</v>
       </c>
@@ -5305,7 +5305,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>84</v>
       </c>
@@ -5313,7 +5313,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>87</v>
       </c>
@@ -5321,7 +5321,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>88</v>
       </c>
@@ -5329,7 +5329,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>91</v>
       </c>
@@ -5337,7 +5337,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>94</v>
       </c>
@@ -5345,7 +5345,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>97</v>
       </c>
@@ -5353,7 +5353,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>100</v>
       </c>
@@ -5361,7 +5361,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>103</v>
       </c>
@@ -5369,7 +5369,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>105</v>
       </c>
@@ -5377,7 +5377,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>108</v>
       </c>
@@ -5385,7 +5385,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>111</v>
       </c>
@@ -5393,7 +5393,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>112</v>
       </c>
@@ -5401,7 +5401,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>115</v>
       </c>
@@ -5409,7 +5409,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>118</v>
       </c>
@@ -5417,7 +5417,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>120</v>
       </c>
@@ -5425,7 +5425,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>123</v>
       </c>
@@ -5433,7 +5433,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>126</v>
       </c>
@@ -5441,7 +5441,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>127</v>
       </c>
@@ -5449,7 +5449,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>130</v>
       </c>
@@ -5457,7 +5457,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>132</v>
       </c>
@@ -5465,7 +5465,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>135</v>
       </c>
@@ -5473,7 +5473,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>138</v>
       </c>
@@ -5481,7 +5481,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>141</v>
       </c>
@@ -5489,7 +5489,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>143</v>
       </c>
@@ -5497,7 +5497,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>146</v>
       </c>
@@ -5505,7 +5505,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>148</v>
       </c>
@@ -5513,7 +5513,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>151</v>
       </c>
@@ -5521,7 +5521,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>154</v>
       </c>
@@ -5529,7 +5529,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>157</v>
       </c>
@@ -5537,7 +5537,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>160</v>
       </c>
@@ -5545,7 +5545,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>163</v>
       </c>
@@ -5553,7 +5553,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>166</v>
       </c>
@@ -5561,7 +5561,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>169</v>
       </c>
@@ -5569,7 +5569,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>172</v>
       </c>
@@ -5577,7 +5577,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>174</v>
       </c>
@@ -5585,7 +5585,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>177</v>
       </c>
@@ -5593,7 +5593,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>180</v>
       </c>
@@ -5601,7 +5601,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>182</v>
       </c>
@@ -5609,7 +5609,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>185</v>
       </c>
@@ -5617,7 +5617,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>188</v>
       </c>
@@ -5625,7 +5625,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>191</v>
       </c>
@@ -5633,7 +5633,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>193</v>
       </c>
@@ -5641,7 +5641,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>196</v>
       </c>

</xml_diff>